<commit_message>
setup all-at-once tester, added final 1k tables
</commit_message>
<xml_diff>
--- a/1k/lat_1k.xlsx
+++ b/1k/lat_1k.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikesog\CorvinusProject\Corvinus\1k\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9224FDCA-9628-4E26-A2F4-D6E925D3AE07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9CB82F1-5E9A-464A-9314-46C54F914A2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{46F7A48C-C0C1-4A99-8267-FB576A2BD9E2}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$1399</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$A$1396</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1398" uniqueCount="1398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1395" uniqueCount="1395">
   <si>
     <t>Adata</t>
   </si>
@@ -240,9 +240,6 @@
     <t>Austriņš</t>
   </si>
   <si>
-    <t>A cont.</t>
-  </si>
-  <si>
     <t>Austrums</t>
   </si>
   <si>
@@ -444,9 +441,6 @@
     <t>Bleijs</t>
   </si>
   <si>
-    <t>B cont.</t>
-  </si>
-  <si>
     <t>Blusiņš</t>
   </si>
   <si>
@@ -844,9 +838,6 @@
   </si>
   <si>
     <t>Dobelnieks</t>
-  </si>
-  <si>
-    <t>D cont.</t>
   </si>
   <si>
     <t>Dombrovskis</t>
@@ -4593,15 +4584,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30532C55-010C-46EC-92DA-7CB18BD00D4E}">
-  <dimension ref="A1:A1398"/>
+  <dimension ref="A1:A1395"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>1397</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.35">
@@ -11574,23 +11567,8 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="1396" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1396" t="s">
-        <v>1394</v>
-      </c>
-    </row>
-    <row r="1397" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1397" t="s">
-        <v>1395</v>
-      </c>
-    </row>
-    <row r="1398" spans="1:1" x14ac:dyDescent="0.35">
-      <c r="A1398" t="s">
-        <v>1396</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:A1399" xr:uid="{30532C55-010C-46EC-92DA-7CB18BD00D4E}"/>
+  <autoFilter ref="A1:A1396" xr:uid="{30532C55-010C-46EC-92DA-7CB18BD00D4E}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>